<commit_message>
Mistake with binning correct
</commit_message>
<xml_diff>
--- a/Spending Analysis 2023/Final.xlsx
+++ b/Spending Analysis 2023/Final.xlsx
@@ -8274,7 +8274,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Transfers</t>
+          <t>Rent &amp; Utilities</t>
         </is>
       </c>
       <c r="C413" s="2" t="n">
@@ -8806,7 +8806,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>Transfers</t>
+          <t>Rent &amp; Utilities</t>
         </is>
       </c>
       <c r="C441" s="2" t="n">
@@ -9376,7 +9376,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>Transfers</t>
+          <t>Rent &amp; Utilities</t>
         </is>
       </c>
       <c r="C471" s="2" t="n">
@@ -10364,7 +10364,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>Transfers</t>
+          <t>Rent &amp; Utilities</t>
         </is>
       </c>
       <c r="C523" s="2" t="n">
@@ -10383,7 +10383,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>Transfers</t>
+          <t>Rent &amp; Utilities</t>
         </is>
       </c>
       <c r="C524" s="2" t="n">

</xml_diff>